<commit_message>
bugfix: Handle exist category in db
</commit_message>
<xml_diff>
--- a/seeders/category/forum.xlsx
+++ b/seeders/category/forum.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Rproject\forum-express\seeders\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Rproject\forum-express\seeders\category\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E12AEE-9F23-4E1B-8B18-F333C75569F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD384AD1-5E9B-4B8D-8A16-372131D81A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DE8E1277-4370-4DA3-B2F0-C7DF42D737BE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>value</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>private</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81275212-E84D-4A51-8E8F-60EE16D7C658}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,6 +442,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>